<commit_message>
fully setup logistic regression
</commit_message>
<xml_diff>
--- a/Data/Predictions/Logistic Regression/Logistic_Regression_Classifier_Predictions_All_Data.xlsx
+++ b/Data/Predictions/Logistic Regression/Logistic_Regression_Classifier_Predictions_All_Data.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SUV_test_orig_train_03788_resized.jpg</t>
+          <t>Sedan_test_orig_test_00697_resized.jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/SUV_test_orig_train_03788_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Sedan_test_orig_test_00697_resized.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/SUV_test_orig_train_03788_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_00697_resized.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -495,49 +495,49 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_train_00198_resized.jpg</t>
+          <t>Sedan_test_orig_test_04302_resized.jpg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_train_00198_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Sedan_test_orig_test_04302_resized.jpg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_train_00198_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_04302_resized.jpg</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_test_04681_resized.jpg</t>
+          <t>Pickup_test_orig_test_07661_resized.jpg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_test_04681_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Pickup_test_orig_test_07661_resized.jpg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_04681_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Pickup_test_orig_test_07661_resized.jpg</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -549,22 +549,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SUV_test_orig_train_05749_resized.jpg</t>
+          <t>SUV_test_orig_test_02156_resized.jpg</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/SUV_test_orig_train_05749_resized.jpg</t>
+          <t>../../../Images/test/Blurred/SUV_test_orig_test_02156_resized.jpg</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/SUV_test_orig_train_05749_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/SUV_test_orig_test_02156_resized.jpg</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_train_02240_resized.jpg</t>
+          <t>Sedan_test_orig_test_01820_resized.jpg</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_train_02240_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Sedan_test_orig_test_01820_resized.jpg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_train_02240_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_01820_resized.jpg</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,54 +598,54 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SUV_test_orig_train_05783_resized.jpg</t>
+          <t>Convertible_test_orig_test_06347_resized.jpg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/SUV_test_orig_train_05783_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Convertible_test_orig_test_06347_resized.jpg</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/SUV_test_orig_train_05783_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Convertible_test_orig_test_06347_resized.jpg</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_train_03876_resized.jpg</t>
+          <t>Pickup_test_orig_test_00858_resized.jpg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_train_03876_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Pickup_test_orig_test_00858_resized.jpg</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_train_03876_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Pickup_test_orig_test_00858_resized.jpg</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -657,22 +657,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SUV_test_orig_test_01271_resized.jpg</t>
+          <t>SUV_test_orig_test_03452_resized.jpg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/SUV_test_orig_test_01271_resized.jpg</t>
+          <t>../../../Images/test/Blurred/SUV_test_orig_test_03452_resized.jpg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/SUV_test_orig_test_01271_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/SUV_test_orig_test_03452_resized.jpg</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -684,44 +684,44 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Pickup_test_orig_test_00485_resized.jpg</t>
+          <t>Pickup_test_orig_train_02871_resized.jpg</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Pickup_test_orig_test_00485_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Pickup_test_orig_train_02871_resized.jpg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Pickup_test_orig_test_00485_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Pickup_test_orig_train_02871_resized.jpg</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SUV_test_orig_test_06761_resized.jpg</t>
+          <t>Sedan_test_orig_test_06356_resized.jpg</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/SUV_test_orig_test_06761_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Sedan_test_orig_test_06356_resized.jpg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/SUV_test_orig_test_06761_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_06356_resized.jpg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -733,49 +733,49 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Convertible_test_orig_test_06645_resized.jpg</t>
+          <t>SUV_test_orig_test_01769_resized.jpg</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Convertible_test_orig_test_06645_resized.jpg</t>
+          <t>../../../Images/test/Blurred/SUV_test_orig_test_01769_resized.jpg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Convertible_test_orig_test_06645_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/SUV_test_orig_test_01769_resized.jpg</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_train_03693_resized.jpg</t>
+          <t>SUV_test_orig_train_03247_resized.jpg</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_train_03693_resized.jpg</t>
+          <t>../../../Images/test/Blurred/SUV_test_orig_train_03247_resized.jpg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_train_03693_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/SUV_test_orig_train_03247_resized.jpg</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -787,27 +787,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sedan_test_orig_test_06408_resized.jpg</t>
+          <t>Pickup_test_orig_test_04440_resized.jpg</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Sedan_test_orig_test_06408_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Pickup_test_orig_test_04440_resized.jpg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Sedan_test_orig_test_06408_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Pickup_test_orig_test_04440_resized.jpg</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -819,17 +819,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pickup_test_orig_test_07302_resized.jpg</t>
+          <t>SUV_test_orig_train_04481_resized.jpg</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Pickup_test_orig_test_07302_resized.jpg</t>
+          <t>../../../Images/test/Blurred/SUV_test_orig_train_04481_resized.jpg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Pickup_test_orig_test_07302_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/SUV_test_orig_train_04481_resized.jpg</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -841,22 +841,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Convertible_test_orig_train_02614_resized.jpg</t>
+          <t>Sedan_test_orig_train_08005_resized.jpg</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>../../../Images/test/Blurred/Convertible_test_orig_train_02614_resized.jpg</t>
+          <t>../../../Images/test/Blurred/Sedan_test_orig_train_08005_resized.jpg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>../../../Images/test/No_Blur/Convertible_test_orig_train_02614_resized.jpg</t>
+          <t>../../../Images/test/No_Blur/Sedan_test_orig_train_08005_resized.jpg</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">

</xml_diff>